<commit_message>
Omitted years from column names. Will specify these via column multi-index
</commit_message>
<xml_diff>
--- a/testExport.xlsx
+++ b/testExport.xlsx
@@ -487,12 +487,12 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>2021 PROJ POS RK</t>
+          <t>PROJ POS RK</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>2021 PROJ PTS</t>
+          <t>PROJ PTS</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
@@ -502,12 +502,12 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>2020 RK</t>
+          <t>RK</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>2020 GP</t>
+          <t>GP</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
@@ -557,7 +557,7 @@
       </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>2020 TTL PTS</t>
+          <t>TTL PTS</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">

</xml_diff>